<commit_message>
new PCA with replicates for physicochemical parameters
</commit_message>
<xml_diff>
--- a/model_results_Aridity_v2.xlsx
+++ b/model_results_Aridity_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugirona-my.sharepoint.com/personal/u4001033_udg_edu/Documents/GRADCATCH/ANALISIS/R/SP_gradient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="856" documentId="8_{8CE68400-0780-4265-B656-84DCEBEF3291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8790639-11A5-4ED8-A65A-44E303636F89}"/>
+  <xr:revisionPtr revIDLastSave="934" documentId="8_{8CE68400-0780-4265-B656-84DCEBEF3291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B4AD07E-C169-47D4-A473-8B19A2D552A2}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{78731C9C-FDD0-4D5D-9F31-25E6ACD05793}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="64">
   <si>
     <t>Model</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>SR:Aridity</t>
+  </si>
+  <si>
+    <t>significance</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -593,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574DAEEA-AE59-4D25-9E92-CE4AB55241EF}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,7 +612,7 @@
     <col min="2" max="2" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,8 +628,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -637,8 +649,11 @@
       <c r="E2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -655,8 +670,11 @@
       <c r="E3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -673,8 +691,11 @@
       <c r="E4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -691,8 +712,11 @@
       <c r="E5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -709,8 +733,11 @@
       <c r="E6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -727,8 +754,11 @@
       <c r="E7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -745,8 +775,11 @@
       <c r="E8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -763,8 +796,11 @@
       <c r="E9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -781,8 +817,11 @@
       <c r="E10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -799,8 +838,11 @@
       <c r="E11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -817,8 +859,11 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -835,8 +880,11 @@
       <c r="E13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -853,8 +901,11 @@
       <c r="E14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -871,8 +922,11 @@
       <c r="E15" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -889,8 +943,11 @@
       <c r="E16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -907,8 +964,11 @@
       <c r="E17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -925,8 +985,11 @@
       <c r="E18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -943,8 +1006,11 @@
       <c r="E19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -961,8 +1027,11 @@
       <c r="E20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -979,8 +1048,11 @@
       <c r="E21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -997,8 +1069,11 @@
       <c r="E22" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1015,8 +1090,11 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1033,8 +1111,11 @@
       <c r="E24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1051,8 +1132,11 @@
       <c r="E25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1069,8 +1153,11 @@
       <c r="E26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1087,8 +1174,11 @@
       <c r="E27" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1105,8 +1195,11 @@
       <c r="E28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1123,8 +1216,11 @@
       <c r="E29" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1141,8 +1237,11 @@
       <c r="E30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1159,8 +1258,11 @@
       <c r="E31" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1177,8 +1279,11 @@
       <c r="E32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1195,8 +1300,11 @@
       <c r="E33" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1213,8 +1321,11 @@
       <c r="E34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1231,8 +1342,11 @@
       <c r="E35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1249,8 +1363,11 @@
       <c r="E36" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1267,8 +1384,11 @@
       <c r="E37" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1285,8 +1405,11 @@
       <c r="E38" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1303,8 +1426,11 @@
       <c r="E39" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1321,8 +1447,11 @@
       <c r="E40" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1339,8 +1468,11 @@
       <c r="E41" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -1357,8 +1489,11 @@
       <c r="E42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -1375,8 +1510,11 @@
       <c r="E43" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -1393,8 +1531,11 @@
       <c r="E44" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -1411,8 +1552,11 @@
       <c r="E45" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1429,8 +1573,11 @@
       <c r="E46" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1447,8 +1594,11 @@
       <c r="E47" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1465,8 +1615,11 @@
       <c r="E48" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -1483,8 +1636,11 @@
       <c r="E49" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -1501,8 +1657,11 @@
       <c r="E50" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -1519,8 +1678,11 @@
       <c r="E51" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -1537,8 +1699,11 @@
       <c r="E52" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -1555,8 +1720,11 @@
       <c r="E53" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -1573,8 +1741,11 @@
       <c r="E54" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -1591,8 +1762,11 @@
       <c r="E55" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -1609,8 +1783,11 @@
       <c r="E56" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -1627,8 +1804,11 @@
       <c r="E57" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -1645,8 +1825,11 @@
       <c r="E58" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -1663,8 +1846,11 @@
       <c r="E59" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>38</v>
       </c>
@@ -1681,8 +1867,11 @@
       <c r="E60" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -1699,8 +1888,11 @@
       <c r="E61" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -1717,8 +1909,11 @@
       <c r="E62" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>38</v>
       </c>
@@ -1735,8 +1930,11 @@
       <c r="E63" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -1752,6 +1950,9 @@
       </c>
       <c r="E64" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="F64" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1771,7 +1972,9 @@
       <c r="E65" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F65" s="1"/>
+      <c r="F65" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
@@ -1790,7 +1993,9 @@
       <c r="E66" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F66" s="1"/>
+      <c r="F66" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
@@ -1809,7 +2014,9 @@
       <c r="E67" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F67" s="1"/>
+      <c r="F67" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
@@ -1828,7 +2035,9 @@
       <c r="E68" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F68" s="1"/>
+      <c r="F68" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
@@ -1847,7 +2056,9 @@
       <c r="E69" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F69" s="1"/>
+      <c r="F69" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
@@ -1866,6 +2077,9 @@
       <c r="E70" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="F70" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
@@ -1884,6 +2098,9 @@
       <c r="E71" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F71" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
@@ -1902,6 +2119,9 @@
       <c r="E72" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F72" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
@@ -1920,6 +2140,9 @@
       <c r="E73" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="F73" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -1938,6 +2161,9 @@
       <c r="E74" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F74" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
@@ -1955,17 +2181,22 @@
       </c>
       <c r="E75" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B76" s="4"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B77" s="4"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B78" s="4"/>

</xml_diff>